<commit_message>
update class for test incorecctly name add class for testing 100 incorectly passwords
</commit_message>
<xml_diff>
--- a/src/tests/java/auth/dev/net/data_files/test_incorrectly_name_acc.xlsx
+++ b/src/tests/java/auth/dev/net/data_files/test_incorrectly_name_acc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="24915" windowHeight="12345" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="24915" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Ukr" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="80">
   <si>
     <t>testName</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Символ . (крапка) не може використовуватися на початку і(або) в кінці</t>
   </si>
   <si>
-    <t xml:space="preserve"> Багаторазове використання символу . (крапка) неможливе</t>
-  </si>
-  <si>
     <t>infoTest</t>
   </si>
   <si>
@@ -253,6 +250,12 @@
   </si>
   <si>
     <t xml:space="preserve"> You can’t leave this empty</t>
+  </si>
+  <si>
+    <t>Багаторазове використання символу . (крапка) неможливе</t>
+  </si>
+  <si>
+    <t>12rest21_finrest21_finrest21_finrest21_fin</t>
   </si>
 </sst>
 </file>
@@ -610,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +636,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -641,7 +644,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -1204,7 +1207,7 @@
         <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D42" t="s">
         <v>53</v>
@@ -1215,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
         <v>55</v>
@@ -1233,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection sqref="A1:D43"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,7 +1259,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1264,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1278,7 +1281,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1292,7 +1295,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1306,7 +1309,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -1320,7 +1323,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1334,7 +1337,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -1348,7 +1351,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -1362,7 +1365,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -1376,7 +1379,7 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -1390,7 +1393,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -1404,7 +1407,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -1418,7 +1421,7 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1432,7 +1435,7 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -1446,7 +1449,7 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
@@ -1460,7 +1463,7 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
@@ -1474,7 +1477,7 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
@@ -1488,7 +1491,7 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
@@ -1502,7 +1505,7 @@
         <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
@@ -1516,7 +1519,7 @@
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
@@ -1530,7 +1533,7 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -1544,7 +1547,7 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
@@ -1558,7 +1561,7 @@
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
@@ -1572,7 +1575,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
@@ -1586,7 +1589,7 @@
         <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
@@ -1600,7 +1603,7 @@
         <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
@@ -1614,7 +1617,7 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
@@ -1628,7 +1631,7 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" t="s">
         <v>15</v>
@@ -1642,7 +1645,7 @@
         <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D29" t="s">
         <v>15</v>
@@ -1656,7 +1659,7 @@
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
         <v>15</v>
@@ -1670,7 +1673,7 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s">
         <v>15</v>
@@ -1684,7 +1687,7 @@
         <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
@@ -1698,7 +1701,7 @@
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D33" t="s">
         <v>15</v>
@@ -1712,7 +1715,7 @@
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
@@ -1726,7 +1729,7 @@
         <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D35" t="s">
         <v>15</v>
@@ -1740,7 +1743,7 @@
         <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D36" t="s">
         <v>15</v>
@@ -1754,7 +1757,7 @@
         <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
@@ -1768,7 +1771,7 @@
         <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -1782,7 +1785,7 @@
         <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
         <v>47</v>
@@ -1796,7 +1799,7 @@
         <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
         <v>50</v>
@@ -1810,7 +1813,7 @@
         <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D41" t="s">
         <v>52</v>
@@ -1824,7 +1827,7 @@
         <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D42" t="s">
         <v>53</v>
@@ -1879,7 +1882,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1887,7 +1890,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1901,7 +1904,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1915,7 +1918,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1929,7 +1932,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -1943,7 +1946,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1957,7 +1960,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -1971,7 +1974,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -1985,7 +1988,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -1999,7 +2002,7 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -2013,7 +2016,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -2027,7 +2030,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -2041,7 +2044,7 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -2055,7 +2058,7 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -2069,7 +2072,7 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
@@ -2083,7 +2086,7 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
@@ -2097,7 +2100,7 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
@@ -2111,7 +2114,7 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
@@ -2125,7 +2128,7 @@
         <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
@@ -2139,7 +2142,7 @@
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
@@ -2153,7 +2156,7 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -2167,7 +2170,7 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
@@ -2181,7 +2184,7 @@
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
@@ -2195,7 +2198,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
@@ -2209,7 +2212,7 @@
         <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
@@ -2223,7 +2226,7 @@
         <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
@@ -2237,7 +2240,7 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
@@ -2251,7 +2254,7 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
         <v>15</v>
@@ -2265,7 +2268,7 @@
         <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" t="s">
         <v>15</v>
@@ -2279,7 +2282,7 @@
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
         <v>15</v>
@@ -2293,7 +2296,7 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D31" t="s">
         <v>15</v>
@@ -2307,7 +2310,7 @@
         <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
@@ -2321,7 +2324,7 @@
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33" t="s">
         <v>15</v>
@@ -2335,7 +2338,7 @@
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
@@ -2349,7 +2352,7 @@
         <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D35" t="s">
         <v>15</v>
@@ -2363,7 +2366,7 @@
         <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D36" t="s">
         <v>15</v>
@@ -2377,7 +2380,7 @@
         <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
@@ -2391,7 +2394,7 @@
         <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -2405,7 +2408,7 @@
         <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D39" t="s">
         <v>47</v>
@@ -2419,7 +2422,7 @@
         <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D40" t="s">
         <v>50</v>
@@ -2433,7 +2436,7 @@
         <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D41" t="s">
         <v>52</v>
@@ -2447,7 +2450,7 @@
         <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D42" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
update and new test: verified forbidden password
</commit_message>
<xml_diff>
--- a/src/tests/java/auth/dev/net/data_files/test_incorrectly_name_acc.xlsx
+++ b/src/tests/java/auth/dev/net/data_files/test_incorrectly_name_acc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="79">
   <si>
     <t>testName</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>infoTest</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>info</t>
@@ -613,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,9 +640,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" t="s">
         <v>58</v>
       </c>
@@ -1207,7 +1202,7 @@
         <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D42" t="s">
         <v>53</v>
@@ -1218,7 +1213,7 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
         <v>55</v>
@@ -1259,7 +1254,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1267,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1281,7 +1276,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1295,7 +1290,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1309,7 +1304,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -1323,7 +1318,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1337,7 +1332,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -1351,7 +1346,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -1365,7 +1360,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -1379,7 +1374,7 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -1393,7 +1388,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -1407,7 +1402,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -1421,7 +1416,7 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1435,7 +1430,7 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -1449,7 +1444,7 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
@@ -1463,7 +1458,7 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
@@ -1477,7 +1472,7 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
@@ -1491,7 +1486,7 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
@@ -1505,7 +1500,7 @@
         <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
@@ -1519,7 +1514,7 @@
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
@@ -1533,7 +1528,7 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -1547,7 +1542,7 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
@@ -1561,7 +1556,7 @@
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
@@ -1575,7 +1570,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
@@ -1589,7 +1584,7 @@
         <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
@@ -1603,7 +1598,7 @@
         <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
@@ -1617,7 +1612,7 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
@@ -1631,7 +1626,7 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
         <v>15</v>
@@ -1645,7 +1640,7 @@
         <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
         <v>15</v>
@@ -1659,7 +1654,7 @@
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30" t="s">
         <v>15</v>
@@ -1673,7 +1668,7 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
         <v>15</v>
@@ -1687,7 +1682,7 @@
         <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
@@ -1701,7 +1696,7 @@
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D33" t="s">
         <v>15</v>
@@ -1715,7 +1710,7 @@
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
@@ -1729,7 +1724,7 @@
         <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D35" t="s">
         <v>15</v>
@@ -1743,7 +1738,7 @@
         <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D36" t="s">
         <v>15</v>
@@ -1757,7 +1752,7 @@
         <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
@@ -1771,7 +1766,7 @@
         <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -1785,7 +1780,7 @@
         <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" t="s">
         <v>47</v>
@@ -1799,7 +1794,7 @@
         <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
         <v>50</v>
@@ -1813,7 +1808,7 @@
         <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D41" t="s">
         <v>52</v>
@@ -1827,7 +1822,7 @@
         <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D42" t="s">
         <v>53</v>
@@ -1882,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1890,7 +1885,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1904,7 +1899,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1918,7 +1913,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1932,7 +1927,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -1946,7 +1941,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1960,7 +1955,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -1974,7 +1969,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -1988,7 +1983,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -2002,7 +1997,7 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -2016,7 +2011,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -2030,7 +2025,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -2044,7 +2039,7 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -2058,7 +2053,7 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -2072,7 +2067,7 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
@@ -2086,7 +2081,7 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
@@ -2100,7 +2095,7 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
@@ -2114,7 +2109,7 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
@@ -2128,7 +2123,7 @@
         <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
@@ -2142,7 +2137,7 @@
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
@@ -2156,7 +2151,7 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -2170,7 +2165,7 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
@@ -2184,7 +2179,7 @@
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
@@ -2198,7 +2193,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
@@ -2212,7 +2207,7 @@
         <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
@@ -2226,7 +2221,7 @@
         <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
@@ -2240,7 +2235,7 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
@@ -2254,7 +2249,7 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
         <v>15</v>
@@ -2268,7 +2263,7 @@
         <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
         <v>15</v>
@@ -2282,7 +2277,7 @@
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D30" t="s">
         <v>15</v>
@@ -2296,7 +2291,7 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" t="s">
         <v>15</v>
@@ -2310,7 +2305,7 @@
         <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
@@ -2324,7 +2319,7 @@
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D33" t="s">
         <v>15</v>
@@ -2338,7 +2333,7 @@
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
@@ -2352,7 +2347,7 @@
         <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D35" t="s">
         <v>15</v>
@@ -2366,7 +2361,7 @@
         <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" t="s">
         <v>15</v>
@@ -2380,7 +2375,7 @@
         <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
@@ -2394,7 +2389,7 @@
         <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -2408,7 +2403,7 @@
         <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D39" t="s">
         <v>47</v>
@@ -2422,7 +2417,7 @@
         <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
         <v>50</v>
@@ -2436,7 +2431,7 @@
         <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D41" t="s">
         <v>52</v>
@@ -2450,7 +2445,7 @@
         <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D42" t="s">
         <v>53</v>

</xml_diff>